<commit_message>
Add Chart to inital results Add weight to Feedback
</commit_message>
<xml_diff>
--- a/InitialResultsv2.xlsx
+++ b/InitialResultsv2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b75b1c6a55d49cb/College/JuniorYear/CS5140/Grade Data Mining Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\North\OneDrive\College\JuniorYear\CS5140\Grade Data Mining Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{2895182A-7C7B-46C6-B047-613BEA9930D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{A85F0232-B279-4E71-8B02-8B74F8FEC351}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{2895182A-7C7B-46C6-B047-613BEA9930D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9C2BBD5B-17B3-4901-93C0-53F2751F79D4}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="2850" windowWidth="26100" windowHeight="16545" xr2:uid="{C2498C7F-B6B4-44DE-9D2A-2A6F06A73C51}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{C2498C7F-B6B4-44DE-9D2A-2A6F06A73C51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,6 +621,1260 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Feedback</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0.5"/>
+            <c:backward val="0.5"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.5802482097145264"/>
+                  <c:y val="0.42994867057424835"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>3.47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.72</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.36</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.51</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.01</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.27</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.58</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.49</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.61</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>2.7189999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.677</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.548</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.532</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4929999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.448</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4409999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.4350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3860000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.335</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.3130000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.29</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.081</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0510000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.032</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.889</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.8660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.829</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.756</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.7270000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.651</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.3129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.2450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.085</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.745</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.63400000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-74BC-4063-AB3F-0A2C03061D2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="962360800"/>
+        <c:axId val="962360472"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="962360800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>GPA</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Given</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="962360472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="962360472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Feedback</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Received</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="962360800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAD86026-8665-4965-9F4D-919424FB3BB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -922,7 +2176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFFCC70A-CE65-4693-B181-9EEFBEA53E63}">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1770,8 +3024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621D1986-EE77-40BD-96CB-454FC5200FFF}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,7 +3062,7 @@
         <v>3.47</v>
       </c>
       <c r="C2">
-        <v>4.7350000000000003</v>
+        <v>2.7189999999999999</v>
       </c>
       <c r="D2" t="s">
         <v>102</v>
@@ -1825,7 +3079,7 @@
         <v>3.19</v>
       </c>
       <c r="C3">
-        <v>4.6959999999999997</v>
+        <v>2.677</v>
       </c>
       <c r="D3" t="s">
         <v>66</v>
@@ -1836,53 +3090,53 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3.86</v>
       </c>
       <c r="C4">
-        <v>4.5709999999999997</v>
+        <v>2.548</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B5">
-        <v>3.86</v>
+        <v>3.06</v>
       </c>
       <c r="C5">
-        <v>4.5590000000000002</v>
+        <v>2.54</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B6">
-        <v>3.06</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>4.5579999999999998</v>
+        <v>2.532</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1893,7 +3147,7 @@
         <v>3.62</v>
       </c>
       <c r="C7">
-        <v>4.5330000000000004</v>
+        <v>2.5049999999999999</v>
       </c>
       <c r="D7" t="s">
         <v>81</v>
@@ -1910,7 +3164,7 @@
         <v>3.13</v>
       </c>
       <c r="C8">
-        <v>4.5250000000000004</v>
+        <v>2.5049999999999999</v>
       </c>
       <c r="D8" t="s">
         <v>94</v>
@@ -1927,7 +3181,7 @@
         <v>3.7</v>
       </c>
       <c r="C9">
-        <v>4.5090000000000003</v>
+        <v>2.4929999999999999</v>
       </c>
       <c r="D9" t="s">
         <v>60</v>
@@ -1944,7 +3198,7 @@
         <v>3.39</v>
       </c>
       <c r="C10">
-        <v>4.4820000000000002</v>
+        <v>2.448</v>
       </c>
       <c r="D10" t="s">
         <v>96</v>
@@ -1955,36 +3209,36 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B11">
-        <v>3.36</v>
+        <v>2.72</v>
       </c>
       <c r="C11">
-        <v>4.4809999999999999</v>
+        <v>2.4409999999999998</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B12">
-        <v>2.72</v>
+        <v>3.36</v>
       </c>
       <c r="C12">
-        <v>4.4770000000000003</v>
+        <v>2.4350000000000001</v>
       </c>
       <c r="D12" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="E12" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1995,7 +3249,7 @@
         <v>3.19</v>
       </c>
       <c r="C13">
-        <v>4.476</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="D13" t="s">
         <v>77</v>
@@ -2012,7 +3266,7 @@
         <v>3.09</v>
       </c>
       <c r="C14">
-        <v>4.4329999999999998</v>
+        <v>2.3860000000000001</v>
       </c>
       <c r="D14" t="s">
         <v>106</v>
@@ -2029,7 +3283,7 @@
         <v>3.51</v>
       </c>
       <c r="C15">
-        <v>4.3849999999999998</v>
+        <v>2.335</v>
       </c>
       <c r="D15" t="s">
         <v>92</v>
@@ -2046,7 +3300,7 @@
         <v>3.01</v>
       </c>
       <c r="C16">
-        <v>4.3559999999999999</v>
+        <v>2.3130000000000002</v>
       </c>
       <c r="D16" t="s">
         <v>79</v>
@@ -2063,7 +3317,7 @@
         <v>3.6</v>
       </c>
       <c r="C17">
-        <v>4.3470000000000004</v>
+        <v>2.29</v>
       </c>
       <c r="D17" t="s">
         <v>56</v>
@@ -2080,7 +3334,7 @@
         <v>3.27</v>
       </c>
       <c r="C18">
-        <v>4.1559999999999997</v>
+        <v>2.081</v>
       </c>
       <c r="D18" t="s">
         <v>100</v>
@@ -2097,7 +3351,7 @@
         <v>3.5</v>
       </c>
       <c r="C19">
-        <v>4.1509999999999998</v>
+        <v>2.0510000000000002</v>
       </c>
       <c r="D19" t="s">
         <v>73</v>
@@ -2114,7 +3368,7 @@
         <v>2.58</v>
       </c>
       <c r="C20">
-        <v>4.1349999999999998</v>
+        <v>2.032</v>
       </c>
       <c r="D20" t="s">
         <v>90</v>
@@ -2131,7 +3385,7 @@
         <v>3.55</v>
       </c>
       <c r="C21">
-        <v>4.0270000000000001</v>
+        <v>1.92</v>
       </c>
       <c r="D21" t="s">
         <v>75</v>
@@ -2148,7 +3402,7 @@
         <v>3.35</v>
       </c>
       <c r="C22">
-        <v>4.0049999999999999</v>
+        <v>1.889</v>
       </c>
       <c r="D22" t="s">
         <v>51</v>
@@ -2165,7 +3419,7 @@
         <v>3.14</v>
       </c>
       <c r="C23">
-        <v>3.992</v>
+        <v>1.8660000000000001</v>
       </c>
       <c r="D23" t="s">
         <v>112</v>
@@ -2182,7 +3436,7 @@
         <v>3.11</v>
       </c>
       <c r="C24">
-        <v>3.97</v>
+        <v>1.829</v>
       </c>
       <c r="D24" t="s">
         <v>104</v>
@@ -2199,7 +3453,7 @@
         <v>3.23</v>
       </c>
       <c r="C25">
-        <v>3.9020000000000001</v>
+        <v>1.756</v>
       </c>
       <c r="D25" t="s">
         <v>57</v>
@@ -2216,7 +3470,7 @@
         <v>3</v>
       </c>
       <c r="C26">
-        <v>3.8679999999999999</v>
+        <v>1.7270000000000001</v>
       </c>
       <c r="D26" t="s">
         <v>71</v>
@@ -2233,7 +3487,7 @@
         <v>3.49</v>
       </c>
       <c r="C27">
-        <v>3.8170000000000002</v>
+        <v>1.651</v>
       </c>
       <c r="D27" t="s">
         <v>64</v>
@@ -2250,7 +3504,7 @@
         <v>3.61</v>
       </c>
       <c r="C28">
-        <v>3.528</v>
+        <v>1.3129999999999999</v>
       </c>
       <c r="D28" t="s">
         <v>110</v>
@@ -2267,7 +3521,7 @@
         <v>2.88</v>
       </c>
       <c r="C29">
-        <v>3.4649999999999999</v>
+        <v>1.2450000000000001</v>
       </c>
       <c r="D29" t="s">
         <v>85</v>
@@ -2284,7 +3538,7 @@
         <v>2.9</v>
       </c>
       <c r="C30">
-        <v>3.339</v>
+        <v>1.085</v>
       </c>
       <c r="D30" t="s">
         <v>55</v>
@@ -2301,7 +3555,7 @@
         <v>2.59</v>
       </c>
       <c r="C31">
-        <v>3.0710000000000002</v>
+        <v>0.745</v>
       </c>
       <c r="D31" t="s">
         <v>62</v>
@@ -2318,7 +3572,7 @@
         <v>3.28</v>
       </c>
       <c r="C32">
-        <v>2.9929999999999999</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="D32" t="s">
         <v>69</v>
@@ -2515,9 +3769,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E43">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E44">
     <sortCondition descending="1" ref="C1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>